<commit_message>
few changes for last task
</commit_message>
<xml_diff>
--- a/src/module6/week5/soapUITask2/DataForCalc.xlsx
+++ b/src/module6/week5/soapUITask2/DataForCalc.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>X</t>
   </si>
@@ -33,6 +33,18 @@
   </si>
   <si>
     <t>result</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>java.rmi.UnmarshalException</t>
+  </si>
+  <si>
+    <t>reg</t>
   </si>
 </sst>
 </file>
@@ -354,13 +366,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="25.21875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -407,6 +422,37 @@
       <c r="C4" s="1">
         <f>A4+B4</f>
         <v>15766</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>-123</v>
+      </c>
+      <c r="B6">
+        <v>123525</v>
+      </c>
+      <c r="C6" s="1">
+        <f>A6+B6</f>
+        <v>123402</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Module7 week 1 hometask added (Logger and screenshot with highlighting)
</commit_message>
<xml_diff>
--- a/src/module6/week5/soapUITask2/DataForCalc.xlsx
+++ b/src/module6/week5/soapUITask2/DataForCalc.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <t>X</t>
   </si>
@@ -44,7 +44,10 @@
     <t>java.rmi.UnmarshalException</t>
   </si>
   <si>
-    <t>reg</t>
+    <t>sdf</t>
+  </si>
+  <si>
+    <t>srg</t>
   </si>
 </sst>
 </file>
@@ -366,10 +369,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -396,7 +399,6 @@
         <v>3</v>
       </c>
       <c r="C2" s="1">
-        <f>A2+B2</f>
         <v>5</v>
       </c>
     </row>
@@ -408,8 +410,7 @@
         <v>56</v>
       </c>
       <c r="C3" s="1">
-        <f>A3+B3</f>
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -448,12 +449,29 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
+      <c r="A7" t="s">
         <v>6</v>
+      </c>
+      <c r="B7">
+        <v>1243</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
       </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>345</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C9" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>